<commit_message>
alteração do sistema para proteger recursos aws e gemini
</commit_message>
<xml_diff>
--- a/dados_vendas_2023.xlsx
+++ b/dados_vendas_2023.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/de69ac21027d344b/CURSOS do PDR/imersao-alura-e-google/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="16" documentId="11_7FF936995BB05B6943793111595ED87656D0C149" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{664ABE71-2A08-416D-80EB-21183438482D}"/>
+  <xr:revisionPtr revIDLastSave="21" documentId="11_7FF936995BB05B6943793111595ED87656D0C149" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3A77DB84-A6DD-4F92-ABC7-90398FD596C9}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,20 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$D$901</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -206,6 +219,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -493,10 +510,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D901"/>
+  <dimension ref="A1:D902"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" topLeftCell="A883" workbookViewId="0">
+      <selection activeCell="B902" sqref="B902"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12070,10 +12087,10 @@
     </row>
     <row r="827" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A827" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="B827">
-        <v>125063</v>
+        <v>40555</v>
       </c>
       <c r="C827" t="s">
         <v>1</v>
@@ -12084,13 +12101,13 @@
     </row>
     <row r="828" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A828" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="B828">
-        <v>74490</v>
+        <v>42636</v>
       </c>
       <c r="C828" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="D828" t="s">
         <v>31</v>
@@ -12098,13 +12115,13 @@
     </row>
     <row r="829" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A829" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B829">
-        <v>224173</v>
+        <v>43746</v>
       </c>
       <c r="C829" t="s">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="D829" t="s">
         <v>31</v>
@@ -12112,10 +12129,10 @@
     </row>
     <row r="830" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A830" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B830">
-        <v>245787</v>
+        <v>46051</v>
       </c>
       <c r="C830" t="s">
         <v>1</v>
@@ -12126,13 +12143,13 @@
     </row>
     <row r="831" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A831" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="B831">
-        <v>40555</v>
+        <v>48187</v>
       </c>
       <c r="C831" t="s">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="D831" t="s">
         <v>31</v>
@@ -12140,13 +12157,13 @@
     </row>
     <row r="832" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A832" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B832">
-        <v>46051</v>
+        <v>53177</v>
       </c>
       <c r="C832" t="s">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="D832" t="s">
         <v>31</v>
@@ -12154,13 +12171,13 @@
     </row>
     <row r="833" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A833" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B833">
-        <v>86496</v>
+        <v>61531</v>
       </c>
       <c r="C833" t="s">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="D833" t="s">
         <v>31</v>
@@ -12168,13 +12185,13 @@
     </row>
     <row r="834" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A834" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="B834">
-        <v>152715</v>
+        <v>70708</v>
       </c>
       <c r="C834" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="D834" t="s">
         <v>31</v>
@@ -12182,13 +12199,13 @@
     </row>
     <row r="835" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A835" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B835">
-        <v>231518</v>
+        <v>71865</v>
       </c>
       <c r="C835" t="s">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="D835" t="s">
         <v>31</v>
@@ -12196,10 +12213,10 @@
     </row>
     <row r="836" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A836" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="B836">
-        <v>288374</v>
+        <v>74490</v>
       </c>
       <c r="C836" t="s">
         <v>1</v>
@@ -12210,13 +12227,13 @@
     </row>
     <row r="837" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A837" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B837">
-        <v>229007</v>
+        <v>79306</v>
       </c>
       <c r="C837" t="s">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="D837" t="s">
         <v>31</v>
@@ -12224,13 +12241,13 @@
     </row>
     <row r="838" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A838" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="B838">
-        <v>237441</v>
+        <v>79544</v>
       </c>
       <c r="C838" t="s">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="D838" t="s">
         <v>31</v>
@@ -12238,13 +12255,13 @@
     </row>
     <row r="839" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A839" t="s">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="B839">
-        <v>86435</v>
+        <v>84012</v>
       </c>
       <c r="C839" t="s">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="D839" t="s">
         <v>31</v>
@@ -12252,13 +12269,13 @@
     </row>
     <row r="840" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A840" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="B840">
-        <v>257827</v>
+        <v>85144</v>
       </c>
       <c r="C840" t="s">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="D840" t="s">
         <v>31</v>
@@ -12266,10 +12283,10 @@
     </row>
     <row r="841" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A841" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B841">
-        <v>284778</v>
+        <v>86435</v>
       </c>
       <c r="C841" t="s">
         <v>1</v>
@@ -12280,13 +12297,13 @@
     </row>
     <row r="842" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A842" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="B842">
-        <v>84012</v>
+        <v>86496</v>
       </c>
       <c r="C842" t="s">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="D842" t="s">
         <v>31</v>
@@ -12294,10 +12311,10 @@
     </row>
     <row r="843" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A843" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B843">
-        <v>270625</v>
+        <v>89276</v>
       </c>
       <c r="C843" t="s">
         <v>17</v>
@@ -12308,13 +12325,13 @@
     </row>
     <row r="844" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A844" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="B844">
-        <v>242946</v>
+        <v>90759</v>
       </c>
       <c r="C844" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D844" t="s">
         <v>31</v>
@@ -12322,13 +12339,13 @@
     </row>
     <row r="845" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A845" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B845">
-        <v>219336</v>
+        <v>94050</v>
       </c>
       <c r="C845" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D845" t="s">
         <v>31</v>
@@ -12336,13 +12353,13 @@
     </row>
     <row r="846" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A846" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B846">
-        <v>89276</v>
+        <v>94964</v>
       </c>
       <c r="C846" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D846" t="s">
         <v>31</v>
@@ -12350,13 +12367,13 @@
     </row>
     <row r="847" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A847" t="s">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="B847">
-        <v>221026</v>
+        <v>95220</v>
       </c>
       <c r="C847" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D847" t="s">
         <v>31</v>
@@ -12364,13 +12381,13 @@
     </row>
     <row r="848" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A848" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="B848">
-        <v>79544</v>
+        <v>95713</v>
       </c>
       <c r="C848" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D848" t="s">
         <v>31</v>
@@ -12378,13 +12395,13 @@
     </row>
     <row r="849" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A849" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="B849">
-        <v>71865</v>
+        <v>108583</v>
       </c>
       <c r="C849" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D849" t="s">
         <v>31</v>
@@ -12392,13 +12409,13 @@
     </row>
     <row r="850" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A850" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="B850">
-        <v>61531</v>
+        <v>112764</v>
       </c>
       <c r="C850" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D850" t="s">
         <v>31</v>
@@ -12406,13 +12423,13 @@
     </row>
     <row r="851" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A851" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B851">
-        <v>239160</v>
+        <v>113181</v>
       </c>
       <c r="C851" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D851" t="s">
         <v>31</v>
@@ -12420,13 +12437,13 @@
     </row>
     <row r="852" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A852" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="B852">
-        <v>201455</v>
+        <v>113409</v>
       </c>
       <c r="C852" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D852" t="s">
         <v>31</v>
@@ -12434,13 +12451,13 @@
     </row>
     <row r="853" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A853" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="B853">
-        <v>79306</v>
+        <v>114035</v>
       </c>
       <c r="C853" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D853" t="s">
         <v>31</v>
@@ -12448,13 +12465,13 @@
     </row>
     <row r="854" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A854" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="B854">
-        <v>192111</v>
+        <v>114274</v>
       </c>
       <c r="C854" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D854" t="s">
         <v>31</v>
@@ -12462,13 +12479,13 @@
     </row>
     <row r="855" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A855" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B855">
-        <v>246139</v>
+        <v>116044</v>
       </c>
       <c r="C855" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D855" t="s">
         <v>31</v>
@@ -12476,13 +12493,13 @@
     </row>
     <row r="856" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A856" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="B856">
-        <v>161613</v>
+        <v>121410</v>
       </c>
       <c r="C856" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D856" t="s">
         <v>31</v>
@@ -12493,10 +12510,10 @@
         <v>0</v>
       </c>
       <c r="B857">
-        <v>168166</v>
+        <v>125063</v>
       </c>
       <c r="C857" t="s">
-        <v>18</v>
+        <v>1</v>
       </c>
       <c r="D857" t="s">
         <v>31</v>
@@ -12504,13 +12521,13 @@
     </row>
     <row r="858" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A858" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="B858">
-        <v>43746</v>
+        <v>128146</v>
       </c>
       <c r="C858" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D858" t="s">
         <v>31</v>
@@ -12518,13 +12535,13 @@
     </row>
     <row r="859" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A859" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B859">
-        <v>152716</v>
+        <v>134607</v>
       </c>
       <c r="C859" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D859" t="s">
         <v>31</v>
@@ -12532,13 +12549,13 @@
     </row>
     <row r="860" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A860" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="B860">
-        <v>53177</v>
+        <v>143377</v>
       </c>
       <c r="C860" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D860" t="s">
         <v>31</v>
@@ -12546,13 +12563,13 @@
     </row>
     <row r="861" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A861" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B861">
-        <v>259470</v>
+        <v>152715</v>
       </c>
       <c r="C861" t="s">
-        <v>18</v>
+        <v>1</v>
       </c>
       <c r="D861" t="s">
         <v>31</v>
@@ -12560,10 +12577,10 @@
     </row>
     <row r="862" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A862" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B862">
-        <v>287241</v>
+        <v>152716</v>
       </c>
       <c r="C862" t="s">
         <v>18</v>
@@ -12574,13 +12591,13 @@
     </row>
     <row r="863" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A863" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B863">
-        <v>114035</v>
+        <v>152948</v>
       </c>
       <c r="C863" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D863" t="s">
         <v>31</v>
@@ -12588,13 +12605,13 @@
     </row>
     <row r="864" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A864" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="B864">
-        <v>121410</v>
+        <v>153920</v>
       </c>
       <c r="C864" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D864" t="s">
         <v>31</v>
@@ -12602,13 +12619,13 @@
     </row>
     <row r="865" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A865" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="B865">
-        <v>259609</v>
+        <v>161613</v>
       </c>
       <c r="C865" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D865" t="s">
         <v>31</v>
@@ -12616,13 +12633,13 @@
     </row>
     <row r="866" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A866" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="B866">
-        <v>170170</v>
+        <v>163897</v>
       </c>
       <c r="C866" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D866" t="s">
         <v>31</v>
@@ -12630,10 +12647,10 @@
     </row>
     <row r="867" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A867" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B867">
-        <v>116044</v>
+        <v>165745</v>
       </c>
       <c r="C867" t="s">
         <v>18</v>
@@ -12644,10 +12661,10 @@
     </row>
     <row r="868" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A868" t="s">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="B868">
-        <v>232335</v>
+        <v>168166</v>
       </c>
       <c r="C868" t="s">
         <v>18</v>
@@ -12658,10 +12675,10 @@
     </row>
     <row r="869" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A869" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B869">
-        <v>264395</v>
+        <v>170170</v>
       </c>
       <c r="C869" t="s">
         <v>18</v>
@@ -12672,13 +12689,13 @@
     </row>
     <row r="870" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A870" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B870">
-        <v>165745</v>
+        <v>176468</v>
       </c>
       <c r="C870" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D870" t="s">
         <v>31</v>
@@ -12686,13 +12703,13 @@
     </row>
     <row r="871" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A871" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B871">
-        <v>48187</v>
+        <v>185611</v>
       </c>
       <c r="C871" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D871" t="s">
         <v>31</v>
@@ -12700,10 +12717,10 @@
     </row>
     <row r="872" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A872" t="s">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="B872">
-        <v>95220</v>
+        <v>186254</v>
       </c>
       <c r="C872" t="s">
         <v>19</v>
@@ -12714,13 +12731,13 @@
     </row>
     <row r="873" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A873" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="B873">
-        <v>112764</v>
+        <v>192111</v>
       </c>
       <c r="C873" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D873" t="s">
         <v>31</v>
@@ -12728,13 +12745,13 @@
     </row>
     <row r="874" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A874" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B874">
-        <v>114274</v>
+        <v>201455</v>
       </c>
       <c r="C874" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D874" t="s">
         <v>31</v>
@@ -12742,10 +12759,10 @@
     </row>
     <row r="875" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A875" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="B875">
-        <v>250305</v>
+        <v>213299</v>
       </c>
       <c r="C875" t="s">
         <v>19</v>
@@ -12756,10 +12773,10 @@
     </row>
     <row r="876" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A876" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="B876">
-        <v>94050</v>
+        <v>214824</v>
       </c>
       <c r="C876" t="s">
         <v>19</v>
@@ -12770,13 +12787,13 @@
     </row>
     <row r="877" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A877" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B877">
-        <v>85144</v>
+        <v>219336</v>
       </c>
       <c r="C877" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D877" t="s">
         <v>31</v>
@@ -12784,13 +12801,13 @@
     </row>
     <row r="878" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A878" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B878">
-        <v>94964</v>
+        <v>221026</v>
       </c>
       <c r="C878" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D878" t="s">
         <v>31</v>
@@ -12798,13 +12815,13 @@
     </row>
     <row r="879" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A879" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="B879">
-        <v>213299</v>
+        <v>224173</v>
       </c>
       <c r="C879" t="s">
-        <v>19</v>
+        <v>1</v>
       </c>
       <c r="D879" t="s">
         <v>31</v>
@@ -12812,13 +12829,13 @@
     </row>
     <row r="880" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A880" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B880">
-        <v>90759</v>
+        <v>229007</v>
       </c>
       <c r="C880" t="s">
-        <v>19</v>
+        <v>1</v>
       </c>
       <c r="D880" t="s">
         <v>31</v>
@@ -12826,13 +12843,13 @@
     </row>
     <row r="881" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A881" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B881">
-        <v>214824</v>
+        <v>231518</v>
       </c>
       <c r="C881" t="s">
-        <v>19</v>
+        <v>1</v>
       </c>
       <c r="D881" t="s">
         <v>31</v>
@@ -12840,13 +12857,13 @@
     </row>
     <row r="882" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A882" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B882">
-        <v>95713</v>
+        <v>232335</v>
       </c>
       <c r="C882" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D882" t="s">
         <v>31</v>
@@ -12857,10 +12874,10 @@
         <v>13</v>
       </c>
       <c r="B883">
-        <v>186254</v>
+        <v>237441</v>
       </c>
       <c r="C883" t="s">
-        <v>19</v>
+        <v>1</v>
       </c>
       <c r="D883" t="s">
         <v>31</v>
@@ -12868,13 +12885,13 @@
     </row>
     <row r="884" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A884" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B884">
-        <v>185611</v>
+        <v>239160</v>
       </c>
       <c r="C884" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D884" t="s">
         <v>31</v>
@@ -12896,13 +12913,13 @@
     </row>
     <row r="886" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A886" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="B886">
-        <v>276146</v>
+        <v>242946</v>
       </c>
       <c r="C886" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D886" t="s">
         <v>31</v>
@@ -12910,13 +12927,13 @@
     </row>
     <row r="887" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A887" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="B887">
-        <v>128146</v>
+        <v>245787</v>
       </c>
       <c r="C887" t="s">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="D887" t="s">
         <v>31</v>
@@ -12924,13 +12941,13 @@
     </row>
     <row r="888" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A888" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="B888">
-        <v>108583</v>
+        <v>246139</v>
       </c>
       <c r="C888" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D888" t="s">
         <v>31</v>
@@ -12955,10 +12972,10 @@
         <v>5</v>
       </c>
       <c r="B890">
-        <v>134607</v>
+        <v>250305</v>
       </c>
       <c r="C890" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D890" t="s">
         <v>31</v>
@@ -12966,13 +12983,13 @@
     </row>
     <row r="891" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A891" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="B891">
-        <v>152948</v>
+        <v>257827</v>
       </c>
       <c r="C891" t="s">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="D891" t="s">
         <v>31</v>
@@ -12980,10 +12997,10 @@
     </row>
     <row r="892" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A892" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="B892">
-        <v>113409</v>
+        <v>258011</v>
       </c>
       <c r="C892" t="s">
         <v>20</v>
@@ -12994,13 +13011,13 @@
     </row>
     <row r="893" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A893" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B893">
-        <v>279124</v>
+        <v>259470</v>
       </c>
       <c r="C893" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D893" t="s">
         <v>31</v>
@@ -13008,13 +13025,13 @@
     </row>
     <row r="894" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A894" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B894">
-        <v>42636</v>
+        <v>259609</v>
       </c>
       <c r="C894" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D894" t="s">
         <v>31</v>
@@ -13022,13 +13039,13 @@
     </row>
     <row r="895" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A895" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="B895">
-        <v>113181</v>
+        <v>264395</v>
       </c>
       <c r="C895" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D895" t="s">
         <v>31</v>
@@ -13036,13 +13053,13 @@
     </row>
     <row r="896" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A896" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="B896">
-        <v>258011</v>
+        <v>270625</v>
       </c>
       <c r="C896" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D896" t="s">
         <v>31</v>
@@ -13050,13 +13067,13 @@
     </row>
     <row r="897" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A897" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="B897">
-        <v>143377</v>
+        <v>276146</v>
       </c>
       <c r="C897" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D897" t="s">
         <v>31</v>
@@ -13064,10 +13081,10 @@
     </row>
     <row r="898" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A898" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="B898">
-        <v>176468</v>
+        <v>279124</v>
       </c>
       <c r="C898" t="s">
         <v>20</v>
@@ -13078,13 +13095,13 @@
     </row>
     <row r="899" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A899" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B899">
-        <v>153920</v>
+        <v>284778</v>
       </c>
       <c r="C899" t="s">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="D899" t="s">
         <v>31</v>
@@ -13092,13 +13109,13 @@
     </row>
     <row r="900" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A900" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="B900">
-        <v>70708</v>
+        <v>287241</v>
       </c>
       <c r="C900" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D900" t="s">
         <v>31</v>
@@ -13106,16 +13123,22 @@
     </row>
     <row r="901" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A901" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="B901">
-        <v>163897</v>
+        <v>288374</v>
       </c>
       <c r="C901" t="s">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="D901" t="s">
         <v>31</v>
+      </c>
+    </row>
+    <row r="902" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B902">
+        <f>SUM(B2:B901)</f>
+        <v>151630882</v>
       </c>
     </row>
   </sheetData>

</xml_diff>